<commit_message>
benerin export excel dengan detailnya
</commit_message>
<xml_diff>
--- a/database/seeders/files/testing.xlsx
+++ b/database/seeders/files/testing.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\BE-Absensi-Siswa\database\seeders\files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F67C22-1D98-4DAB-AA3D-81D2F861D5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>nisn</t>
   </si>
@@ -58,31 +49,39 @@
     <t>Fauzan123</t>
   </si>
   <si>
-    <t>Ahmad Zidan</t>
-  </si>
-  <si>
-    <t>zidan</t>
-  </si>
-  <si>
-    <t>Zidan456</t>
-  </si>
-  <si>
-    <t>ADMIN</t>
+    <t>guru matematika</t>
+  </si>
+  <si>
+    <t>bufit</t>
+  </si>
+  <si>
+    <t>ireireir</t>
+  </si>
+  <si>
+    <t>Guru</t>
+  </si>
+  <si>
+    <t>Alvin Ganteng</t>
+  </si>
+  <si>
+    <t>Alvin</t>
+  </si>
+  <si>
+    <t>Anton</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="2">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -93,43 +92,40 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -319,25 +315,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="18.13"/>
+    <col customWidth="1" min="2" max="2" width="22.25"/>
+    <col customWidth="1" min="3" max="3" width="18.63"/>
+    <col customWidth="1" min="4" max="4" width="17.38"/>
+    <col customWidth="1" min="5" max="5" width="16.0"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -354,9 +352,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="1">
-        <v>129385</v>
+        <v>129385.0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -371,9 +369,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" s="1">
-        <v>92831</v>
+        <v>92831.0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -388,9 +386,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>654321</v>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>2832083.0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
@@ -405,7 +403,41 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>12345.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1">
+        <v>12345.0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>54321.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1">
+        <v>12345.0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ini benerin response login
</commit_message>
<xml_diff>
--- a/database/seeders/files/testing.xlsx
+++ b/database/seeders/files/testing.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>nisn</t>
   </si>
@@ -68,6 +68,21 @@
   </si>
   <si>
     <t>Anton</t>
+  </si>
+  <si>
+    <t>HIJRI</t>
+  </si>
+  <si>
+    <t>LENA</t>
+  </si>
+  <si>
+    <t>XI-MM-2</t>
+  </si>
+  <si>
+    <t>NIH</t>
+  </si>
+  <si>
+    <t>X-LPB-2</t>
   </si>
 </sst>
 </file>
@@ -331,8 +346,7 @@
     <col customWidth="1" min="1" max="1" width="18.13"/>
     <col customWidth="1" min="2" max="2" width="22.25"/>
     <col customWidth="1" min="3" max="3" width="18.63"/>
-    <col customWidth="1" min="4" max="4" width="17.38"/>
-    <col customWidth="1" min="5" max="5" width="16.0"/>
+    <col customWidth="1" min="4" max="5" width="16.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -437,6 +451,40 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>21357.0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1">
+        <v>123.0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>213.0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>232.0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1">
+        <v>123.0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>